<commit_message>
chore: update gpa cdv
</commit_message>
<xml_diff>
--- a/Kusal_Data_Set.xlsx
+++ b/Kusal_Data_Set.xlsx
@@ -1,34 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Educational\Project\course-finder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981E91C6-B33C-4A73-92AB-86934A72A1CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF26782-A35C-4DCD-A8E6-CDC4CC4A8631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form responses 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -62,12 +49,6 @@
     <t>NIBM</t>
   </si>
   <si>
-    <t>A/L Stream</t>
-  </si>
-  <si>
-    <t>z-Core</t>
-  </si>
-  <si>
     <t>Interactive Media</t>
   </si>
   <si>
@@ -89,10 +70,16 @@
     <t>University</t>
   </si>
   <si>
-    <t>pecialization (Only for IT graduates/undergraduates)</t>
+    <t>Specialization</t>
   </si>
   <si>
-    <t>What is your GPA if you are a graduating student?2</t>
+    <t>Stream</t>
+  </si>
+  <si>
+    <t>z_core</t>
+  </si>
+  <si>
+    <t>gpa</t>
   </si>
 </sst>
 </file>
@@ -110,6 +97,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -280,10 +268,10 @@
   <autoFilter ref="A1:E505" xr:uid="{27FC18F2-0095-44BA-9648-5E164EC0F77C}"/>
   <tableColumns count="5">
     <tableColumn id="4" xr3:uid="{C6F9AF65-CB48-4EC0-8B2A-27E7557C6A9A}" name="University" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{CF60D45D-BC7C-454C-98E5-0B0224AFDB10}" name="pecialization (Only for IT graduates/undergraduates)" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{9BA60FD3-7668-4F38-A83E-9F348453F55F}" name="A/L Stream" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{EA650479-C2CA-49E4-91FF-C5B96D9C7FE9}" name="z-Core" dataDxfId="1"/>
-    <tableColumn id="1" xr3:uid="{CFAECDC8-3225-44A5-B437-B09164EA94CB}" name="What is your GPA if you are a graduating student?2" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{CF60D45D-BC7C-454C-98E5-0B0224AFDB10}" name="Specialization" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{9BA60FD3-7668-4F38-A83E-9F348453F55F}" name="Stream" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{EA650479-C2CA-49E4-91FF-C5B96D9C7FE9}" name="z_core" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{CFAECDC8-3225-44A5-B437-B09164EA94CB}" name="gpa" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -492,7 +480,7 @@
   </sheetPr>
   <dimension ref="A1:E505"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
@@ -516,16 +504,16 @@
   <sheetData>
     <row r="1" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>19</v>
@@ -539,7 +527,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1">
         <v>0.46779999999999999</v>
@@ -556,7 +544,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1">
         <v>0.92320000000000002</v>
@@ -573,7 +561,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1">
         <v>0.46779999999999999</v>
@@ -590,7 +578,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1">
         <v>0.92320000000000002</v>
@@ -607,7 +595,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1">
         <v>1.0678000000000001</v>
@@ -624,7 +612,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1">
         <v>0.23139999999999999</v>
@@ -641,7 +629,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D8" s="1">
         <v>0.92320000000000002</v>
@@ -658,7 +646,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D9" s="1">
         <v>0.92320000000000002</v>
@@ -675,7 +663,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D10" s="1">
         <v>0.64559999999999995</v>
@@ -692,7 +680,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D11" s="1">
         <v>0.1241</v>
@@ -709,7 +697,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D12" s="1">
         <v>0.92320000000000002</v>
@@ -726,7 +714,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D13" s="1">
         <v>0.92320000000000002</v>
@@ -743,7 +731,7 @@
         <v>3</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D14" s="1">
         <v>0.92320000000000002</v>
@@ -760,7 +748,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D15" s="1">
         <v>0.92320000000000002</v>
@@ -777,7 +765,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D16" s="1">
         <v>0.63560000000000005</v>
@@ -794,7 +782,7 @@
         <v>6</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D17" s="1">
         <v>0.63560000000000005</v>
@@ -811,7 +799,7 @@
         <v>5</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D18" s="1">
         <v>0.63560000000000005</v>
@@ -828,7 +816,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D19" s="1">
         <v>1.1241000000000001</v>
@@ -845,7 +833,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D20" s="1">
         <v>0.1241</v>
@@ -862,7 +850,7 @@
         <v>5</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D21" s="1">
         <v>0.63560000000000005</v>
@@ -879,7 +867,7 @@
         <v>3</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D22">
         <v>0.59230000000000005</v>
@@ -896,7 +884,7 @@
         <v>2</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D23" s="1">
         <v>0.65669999999999995</v>
@@ -913,7 +901,7 @@
         <v>5</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D24" s="1">
         <v>0.63560000000000005</v>
@@ -930,7 +918,7 @@
         <v>7</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D25" s="1">
         <v>0.63560000000000005</v>
@@ -947,7 +935,7 @@
         <v>2</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D26" s="1">
         <v>0.77949999999999997</v>
@@ -964,7 +952,7 @@
         <v>3</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D27" s="1">
         <v>0.77949999999999997</v>
@@ -981,7 +969,7 @@
         <v>5</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D28" s="1">
         <v>0.63560000000000005</v>
@@ -998,7 +986,7 @@
         <v>5</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D29" s="1">
         <v>0.84560000000000002</v>
@@ -1015,7 +1003,7 @@
         <v>7</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D30" s="1">
         <v>0.84560000000000002</v>
@@ -1032,7 +1020,7 @@
         <v>3</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D31" s="1">
         <v>0.77949999999999997</v>
@@ -1049,7 +1037,7 @@
         <v>6</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D32" s="1">
         <v>0.5323</v>
@@ -1066,7 +1054,7 @@
         <v>6</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D33" s="1">
         <v>0.5323</v>
@@ -1083,7 +1071,7 @@
         <v>2</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D34" s="1">
         <v>0.5323</v>
@@ -1100,7 +1088,7 @@
         <v>6</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D35" s="1">
         <v>0.5323</v>
@@ -1117,7 +1105,7 @@
         <v>2</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D36" s="1">
         <v>0.5323</v>
@@ -1134,7 +1122,7 @@
         <v>3</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D37" s="1">
         <v>0.5323</v>
@@ -1151,7 +1139,7 @@
         <v>6</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D38" s="1">
         <v>0.23449999999999999</v>
@@ -1168,7 +1156,7 @@
         <v>5</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D39" s="1">
         <v>0.84560000000000002</v>
@@ -1185,7 +1173,7 @@
         <v>3</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D40" s="1">
         <v>0.23449999999999999</v>
@@ -1202,7 +1190,7 @@
         <v>1</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D41" s="1">
         <v>0.23949999999999999</v>
@@ -1219,7 +1207,7 @@
         <v>1</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D42" s="1">
         <v>0.23949999999999999</v>
@@ -1236,7 +1224,7 @@
         <v>5</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D43" s="1">
         <v>0.84560000000000002</v>
@@ -1253,7 +1241,7 @@
         <v>5</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D44" s="1">
         <v>0.84560000000000002</v>
@@ -1270,7 +1258,7 @@
         <v>2</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D45" s="1">
         <v>0.23449999999999999</v>
@@ -1287,7 +1275,7 @@
         <v>2</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D46" s="1">
         <v>0.23449999999999999</v>
@@ -1304,7 +1292,7 @@
         <v>2</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D47" s="1">
         <v>0.23449999999999999</v>
@@ -1321,7 +1309,7 @@
         <v>2</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D48" s="1">
         <v>0.23449999999999999</v>
@@ -1338,7 +1326,7 @@
         <v>7</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D49" s="1">
         <v>0.84560000000000002</v>
@@ -1355,7 +1343,7 @@
         <v>1</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D50" s="1">
         <v>0.23949999999999999</v>
@@ -1372,7 +1360,7 @@
         <v>5</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D51" s="1">
         <v>0.84560000000000002</v>
@@ -1389,7 +1377,7 @@
         <v>2</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D52" s="1">
         <v>0.23449999999999999</v>
@@ -1406,7 +1394,7 @@
         <v>2</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D53" s="1">
         <v>0.23449999999999999</v>
@@ -1423,7 +1411,7 @@
         <v>2</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D54" s="1">
         <v>0.23449999999999999</v>
@@ -1440,7 +1428,7 @@
         <v>1</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D55" s="1">
         <v>0.23949999999999999</v>
@@ -1457,7 +1445,7 @@
         <v>5</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D56" s="1">
         <v>0.65429999999999999</v>
@@ -1474,7 +1462,7 @@
         <v>5</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D57" s="1">
         <v>1.3867</v>
@@ -1491,7 +1479,7 @@
         <v>7</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D58" s="1">
         <v>0.84560000000000002</v>
@@ -1508,7 +1496,7 @@
         <v>2</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D59" s="1">
         <v>0.23449999999999999</v>
@@ -1525,7 +1513,7 @@
         <v>3</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D60" s="1">
         <v>0.23449999999999999</v>
@@ -1542,7 +1530,7 @@
         <v>5</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D61" s="1">
         <v>1.0056</v>
@@ -1559,7 +1547,7 @@
         <v>2</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D62" s="1">
         <v>0.23449999999999999</v>
@@ -1576,7 +1564,7 @@
         <v>2</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D63" s="1">
         <v>0.23449999999999999</v>
@@ -1593,7 +1581,7 @@
         <v>2</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D64" s="1">
         <v>0.23449999999999999</v>
@@ -1610,7 +1598,7 @@
         <v>2</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D65" s="1">
         <v>0.23449999999999999</v>
@@ -1627,7 +1615,7 @@
         <v>3</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D66" s="1">
         <v>0.23449999999999999</v>
@@ -1644,7 +1632,7 @@
         <v>2</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D67" s="1">
         <v>0.23449999999999999</v>
@@ -1661,7 +1649,7 @@
         <v>2</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D68" s="1">
         <v>0.23449999999999999</v>
@@ -1678,7 +1666,7 @@
         <v>2</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D69" s="1">
         <v>0.23449999999999999</v>
@@ -1695,7 +1683,7 @@
         <v>2</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D70" s="1">
         <v>0.23449999999999999</v>
@@ -1712,7 +1700,7 @@
         <v>3</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D71" s="1">
         <v>0.23449999999999999</v>
@@ -1729,7 +1717,7 @@
         <v>2</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D72" s="1">
         <v>0.23449999999999999</v>
@@ -1746,7 +1734,7 @@
         <v>2</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D73" s="1">
         <v>0.23449999999999999</v>
@@ -1763,7 +1751,7 @@
         <v>3</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D74" s="1">
         <v>0.84560000000000002</v>
@@ -1780,7 +1768,7 @@
         <v>3</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D75" s="1">
         <v>0.84560000000000002</v>
@@ -1797,7 +1785,7 @@
         <v>3</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D76" s="1">
         <v>0.84560000000000002</v>
@@ -1814,7 +1802,7 @@
         <v>3</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D77" s="1">
         <v>0.84560000000000002</v>
@@ -1831,7 +1819,7 @@
         <v>3</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D78" s="1">
         <v>1.1023000000000001</v>
@@ -1848,7 +1836,7 @@
         <v>3</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D79" s="1">
         <v>1.1023000000000001</v>
@@ -1865,7 +1853,7 @@
         <v>3</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D80" s="1">
         <v>1.1023000000000001</v>
@@ -1882,7 +1870,7 @@
         <v>3</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D81" s="1">
         <v>1.1023000000000001</v>
@@ -1899,7 +1887,7 @@
         <v>2</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D82" s="1">
         <v>0.23449999999999999</v>
@@ -1916,7 +1904,7 @@
         <v>2</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D83" s="1">
         <v>1.1023000000000001</v>
@@ -1933,7 +1921,7 @@
         <v>2</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D84" s="1">
         <v>1.1023000000000001</v>
@@ -1950,7 +1938,7 @@
         <v>2</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D85" s="1">
         <v>1.1023000000000001</v>
@@ -1967,7 +1955,7 @@
         <v>3</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D86" s="1">
         <v>1.0032000000000001</v>
@@ -1984,7 +1972,7 @@
         <v>7</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D87" s="1">
         <v>1.0032000000000001</v>
@@ -2001,7 +1989,7 @@
         <v>7</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D88" s="1">
         <v>1.0032000000000001</v>
@@ -2018,7 +2006,7 @@
         <v>7</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D89" s="1">
         <v>1.0032000000000001</v>
@@ -2035,7 +2023,7 @@
         <v>7</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D90" s="1">
         <v>1.0032000000000001</v>
@@ -2052,7 +2040,7 @@
         <v>7</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D91" s="1">
         <v>1.0032000000000001</v>
@@ -2069,7 +2057,7 @@
         <v>7</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D92" s="1">
         <v>0.74350000000000005</v>
@@ -2086,7 +2074,7 @@
         <v>7</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D93" s="1">
         <v>0.74350000000000005</v>
@@ -2103,7 +2091,7 @@
         <v>7</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D94" s="1">
         <v>0.74350000000000005</v>
@@ -2120,7 +2108,7 @@
         <v>7</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D95" s="1">
         <v>0.74350000000000005</v>
@@ -2137,7 +2125,7 @@
         <v>7</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D96" s="1">
         <v>0.74350000000000005</v>
@@ -2154,7 +2142,7 @@
         <v>3</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D97" s="1">
         <v>0.74350000000000005</v>
@@ -2171,7 +2159,7 @@
         <v>7</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D98" s="1">
         <v>0.74350000000000005</v>
@@ -2188,7 +2176,7 @@
         <v>7</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D99" s="1">
         <v>0.74350000000000005</v>
@@ -2205,7 +2193,7 @@
         <v>7</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D100" s="1">
         <v>0.74350000000000005</v>
@@ -2222,7 +2210,7 @@
         <v>7</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D101" s="1">
         <v>0.87690000000000001</v>
@@ -2239,7 +2227,7 @@
         <v>7</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D102" s="1">
         <v>0.87690000000000001</v>
@@ -2256,7 +2244,7 @@
         <v>6</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D103" s="1">
         <v>0.87690000000000001</v>
@@ -2273,7 +2261,7 @@
         <v>7</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D104" s="1">
         <v>0.87690000000000001</v>
@@ -2290,7 +2278,7 @@
         <v>5</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D105" s="1">
         <v>1.0156000000000001</v>
@@ -2307,7 +2295,7 @@
         <v>7</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D106" s="1">
         <v>0.87949999999999995</v>
@@ -2324,7 +2312,7 @@
         <v>3</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D107" s="1">
         <v>0.87690000000000001</v>
@@ -2341,7 +2329,7 @@
         <v>7</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D108" s="1">
         <v>0.12839999999999999</v>
@@ -2358,7 +2346,7 @@
         <v>7</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D109" s="1">
         <v>0.67889999999999995</v>
@@ -2375,7 +2363,7 @@
         <v>7</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D110" s="1">
         <v>0.92559999999999998</v>
@@ -2392,7 +2380,7 @@
         <v>7</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D111" s="1">
         <v>0.14319999999999999</v>
@@ -2409,7 +2397,7 @@
         <v>5</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D112" s="1">
         <v>0.54669999999999996</v>
@@ -2426,7 +2414,7 @@
         <v>7</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D113" s="1">
         <v>0.54669999999999996</v>
@@ -2443,7 +2431,7 @@
         <v>7</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D114" s="1">
         <v>0.76890000000000003</v>
@@ -2460,7 +2448,7 @@
         <v>7</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D115" s="1">
         <v>0.87690000000000001</v>
@@ -2477,7 +2465,7 @@
         <v>7</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D116" s="1">
         <v>0.98670000000000002</v>
@@ -2494,7 +2482,7 @@
         <v>7</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D117" s="1">
         <v>0.98670000000000002</v>
@@ -2511,7 +2499,7 @@
         <v>7</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D118" s="1">
         <v>0.98670000000000002</v>
@@ -2528,7 +2516,7 @@
         <v>7</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D119" s="1">
         <v>0.98670000000000002</v>
@@ -2545,7 +2533,7 @@
         <v>7</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D120" s="1">
         <v>0.98670000000000002</v>
@@ -2562,7 +2550,7 @@
         <v>2</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D121" s="1">
         <v>0.98670000000000002</v>
@@ -2579,7 +2567,7 @@
         <v>6</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D122" s="1">
         <v>0.98670000000000002</v>
@@ -2596,7 +2584,7 @@
         <v>3</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D123" s="1">
         <v>0.98670000000000002</v>
@@ -2613,7 +2601,7 @@
         <v>5</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D124" s="1">
         <v>0.78949999999999998</v>
@@ -2630,7 +2618,7 @@
         <v>5</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D125" s="1">
         <v>0.78949999999999998</v>
@@ -2647,7 +2635,7 @@
         <v>5</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D126" s="1">
         <v>1.2364999999999999</v>
@@ -2664,7 +2652,7 @@
         <v>3</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D127" s="1">
         <v>0.98670000000000002</v>
@@ -2681,7 +2669,7 @@
         <v>3</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D128" s="1">
         <v>0.98670000000000002</v>
@@ -2698,7 +2686,7 @@
         <v>7</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D129" s="1">
         <v>0.98670000000000002</v>
@@ -2715,7 +2703,7 @@
         <v>7</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D130" s="1">
         <v>0.98670000000000002</v>
@@ -2732,7 +2720,7 @@
         <v>7</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D131" s="1">
         <v>0.98670000000000002</v>
@@ -2749,7 +2737,7 @@
         <v>7</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D132" s="1">
         <v>0.98670000000000002</v>
@@ -2766,7 +2754,7 @@
         <v>7</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D133" s="1">
         <v>0.98670000000000002</v>
@@ -2783,7 +2771,7 @@
         <v>7</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D134" s="1">
         <v>0.98670000000000002</v>
@@ -2800,7 +2788,7 @@
         <v>7</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D135" s="1">
         <v>0.98670000000000002</v>
@@ -2817,7 +2805,7 @@
         <v>7</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D136" s="1">
         <v>0.98670000000000002</v>
@@ -2834,7 +2822,7 @@
         <v>7</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D137" s="1">
         <v>0.98670000000000002</v>
@@ -2851,7 +2839,7 @@
         <v>7</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D138" s="1">
         <v>0.98670000000000002</v>
@@ -2868,7 +2856,7 @@
         <v>7</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D139" s="1">
         <v>0.98670000000000002</v>
@@ -2885,7 +2873,7 @@
         <v>7</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D140" s="1">
         <v>0.98670000000000002</v>
@@ -2902,7 +2890,7 @@
         <v>7</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D141" s="1">
         <v>0.94530000000000003</v>
@@ -2919,7 +2907,7 @@
         <v>3</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D142" s="1">
         <v>0.14649999999999999</v>
@@ -2936,7 +2924,7 @@
         <v>3</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D143" s="1">
         <v>0.23449999999999999</v>
@@ -2953,7 +2941,7 @@
         <v>2</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D144" s="1">
         <v>0.94530000000000003</v>
@@ -2970,7 +2958,7 @@
         <v>2</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D145" s="1">
         <v>0.94530000000000003</v>
@@ -2987,7 +2975,7 @@
         <v>3</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D146" s="1">
         <v>0.23150000000000001</v>
@@ -3004,7 +2992,7 @@
         <v>3</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D147" s="1">
         <v>0.23549999999999999</v>
@@ -3021,7 +3009,7 @@
         <v>7</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D148" s="1">
         <v>0.94530000000000003</v>
@@ -3038,7 +3026,7 @@
         <v>3</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D149" s="1">
         <v>0.23749999999999999</v>
@@ -3055,7 +3043,7 @@
         <v>7</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D150" s="1">
         <v>0.94530000000000003</v>
@@ -3072,7 +3060,7 @@
         <v>7</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D151" s="1">
         <v>0.94530000000000003</v>
@@ -3089,7 +3077,7 @@
         <v>3</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D152" s="1">
         <v>0.23050000000000001</v>
@@ -3106,7 +3094,7 @@
         <v>7</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D153" s="1">
         <v>0.94530000000000003</v>
@@ -3123,7 +3111,7 @@
         <v>7</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D154" s="1">
         <v>0.94530000000000003</v>
@@ -3140,7 +3128,7 @@
         <v>7</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D155" s="1">
         <v>0.94530000000000003</v>
@@ -3157,7 +3145,7 @@
         <v>7</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D156" s="1">
         <v>0.94530000000000003</v>
@@ -3174,7 +3162,7 @@
         <v>7</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D157" s="1">
         <v>0.94530000000000003</v>
@@ -3191,7 +3179,7 @@
         <v>7</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D158" s="1">
         <v>0.94530000000000003</v>
@@ -3208,7 +3196,7 @@
         <v>7</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D159" s="1">
         <v>0.91979999999999995</v>
@@ -3225,7 +3213,7 @@
         <v>7</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D160" s="1">
         <v>0.54100000000000004</v>
@@ -3242,7 +3230,7 @@
         <v>2</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D161" s="1">
         <v>0.92879999999999996</v>
@@ -3259,7 +3247,7 @@
         <v>6</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D162" s="1">
         <v>0.94530000000000003</v>
@@ -3276,7 +3264,7 @@
         <v>3</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D163" s="1">
         <v>0.23139999999999999</v>
@@ -3293,7 +3281,7 @@
         <v>5</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D164" s="1">
         <v>0.54210000000000003</v>
@@ -3310,7 +3298,7 @@
         <v>5</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D165" s="1">
         <v>0.95879999999999999</v>
@@ -3327,7 +3315,7 @@
         <v>5</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D166" s="1">
         <v>0.23449999999999999</v>
@@ -3344,7 +3332,7 @@
         <v>3</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D167" s="1">
         <v>0.94530000000000003</v>
@@ -3361,7 +3349,7 @@
         <v>3</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D168" s="1">
         <v>0.94530000000000003</v>
@@ -3378,7 +3366,7 @@
         <v>7</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D169" s="1">
         <v>0.51880000000000004</v>
@@ -3395,7 +3383,7 @@
         <v>7</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D170" s="1">
         <v>0.65890000000000004</v>
@@ -3412,7 +3400,7 @@
         <v>7</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D171" s="1">
         <v>0.85640000000000005</v>
@@ -3429,7 +3417,7 @@
         <v>7</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D172" s="1">
         <v>0.78449999999999998</v>
@@ -3446,7 +3434,7 @@
         <v>3</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D173" s="1">
         <v>0.78049999999999997</v>
@@ -3463,7 +3451,7 @@
         <v>7</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D174" s="1">
         <v>0.6754</v>
@@ -3480,7 +3468,7 @@
         <v>7</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D175" s="1">
         <v>0.91990000000000005</v>
@@ -3497,7 +3485,7 @@
         <v>7</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D176" s="1">
         <v>0.94530000000000003</v>
@@ -3514,7 +3502,7 @@
         <v>3</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D177" s="1">
         <v>0.94530000000000003</v>
@@ -3531,7 +3519,7 @@
         <v>7</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D178" s="1">
         <v>0.87560000000000004</v>
@@ -3548,7 +3536,7 @@
         <v>7</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D179" s="1">
         <v>0.87560000000000004</v>
@@ -3565,7 +3553,7 @@
         <v>7</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D180" s="1">
         <v>0.87560000000000004</v>
@@ -3582,7 +3570,7 @@
         <v>7</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D181" s="1">
         <v>0.87560000000000004</v>
@@ -3599,7 +3587,7 @@
         <v>2</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D182" s="1">
         <v>0.91080000000000005</v>
@@ -3616,7 +3604,7 @@
         <v>1</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D183" s="1">
         <v>1.2395</v>
@@ -3633,7 +3621,7 @@
         <v>2</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D184" s="1">
         <v>0.32450000000000001</v>
@@ -3650,7 +3638,7 @@
         <v>2</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D185" s="1">
         <v>0.90880000000000005</v>
@@ -3667,7 +3655,7 @@
         <v>6</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D186" s="1">
         <v>0.87560000000000004</v>
@@ -3684,7 +3672,7 @@
         <v>3</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D187" s="1">
         <v>0.23449999999999999</v>
@@ -3701,7 +3689,7 @@
         <v>2</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D188" s="1">
         <v>0.90580000000000005</v>
@@ -3718,7 +3706,7 @@
         <v>2</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D189" s="1">
         <v>0.90280000000000005</v>
@@ -3735,7 +3723,7 @@
         <v>2</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D190" s="1">
         <v>0.91879999999999995</v>
@@ -3752,7 +3740,7 @@
         <v>7</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D191" s="1">
         <v>0.87560000000000004</v>
@@ -3769,7 +3757,7 @@
         <v>1</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D192" s="1">
         <v>1.2395</v>
@@ -3786,7 +3774,7 @@
         <v>2</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D193" s="1">
         <v>0.87560000000000004</v>
@@ -3803,7 +3791,7 @@
         <v>1</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D194" s="1">
         <v>0.23949999999999999</v>
@@ -3820,7 +3808,7 @@
         <v>3</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D195" s="1">
         <v>0.87560000000000004</v>
@@ -3837,7 +3825,7 @@
         <v>1</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D196" s="1">
         <v>0.87560000000000004</v>
@@ -3854,7 +3842,7 @@
         <v>1</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D197" s="1">
         <v>0.14560000000000001</v>
@@ -3871,7 +3859,7 @@
         <v>2</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D198" s="1">
         <v>0.87560000000000004</v>
@@ -3888,7 +3876,7 @@
         <v>5</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D199" s="1">
         <v>0.76890000000000003</v>
@@ -3905,7 +3893,7 @@
         <v>1</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D200" s="1">
         <v>0.14560000000000001</v>
@@ -3922,7 +3910,7 @@
         <v>1</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D201" s="1">
         <v>0.46779999999999999</v>
@@ -3939,7 +3927,7 @@
         <v>2</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D202" s="1">
         <v>0.87560000000000004</v>
@@ -3956,7 +3944,7 @@
         <v>6</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D203" s="1">
         <v>0.7893</v>
@@ -3973,7 +3961,7 @@
         <v>5</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D204" s="1">
         <v>0.34560000000000002</v>
@@ -3990,7 +3978,7 @@
         <v>2</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D205" s="1">
         <v>0.7893</v>
@@ -4007,7 +3995,7 @@
         <v>3</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D206" s="1">
         <v>0.7893</v>
@@ -4024,7 +4012,7 @@
         <v>6</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D207" s="1">
         <v>0.7893</v>
@@ -4041,7 +4029,7 @@
         <v>5</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D208" s="1">
         <v>0.24560000000000001</v>
@@ -4058,7 +4046,7 @@
         <v>1</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D209" s="1">
         <v>0.32450000000000001</v>
@@ -4075,7 +4063,7 @@
         <v>3</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D210" s="1">
         <v>0.7893</v>
@@ -4092,7 +4080,7 @@
         <v>5</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D211" s="1">
         <v>0.13239999999999999</v>
@@ -4109,7 +4097,7 @@
         <v>5</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D212" s="1">
         <v>0.23139999999999999</v>
@@ -4126,7 +4114,7 @@
         <v>2</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D213" s="1">
         <v>0.7893</v>
@@ -4143,7 +4131,7 @@
         <v>5</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D214" s="1">
         <v>0.23139999999999999</v>
@@ -4160,7 +4148,7 @@
         <v>7</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D215" s="1">
         <v>0.7893</v>
@@ -4177,7 +4165,7 @@
         <v>2</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D216" s="1">
         <v>0.7893</v>
@@ -4194,7 +4182,7 @@
         <v>5</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D217" s="1">
         <v>0.78539999999999999</v>
@@ -4211,7 +4199,7 @@
         <v>5</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D218" s="1">
         <v>0.78539999999999999</v>
@@ -4228,7 +4216,7 @@
         <v>5</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D219" s="1">
         <v>0.78539999999999999</v>
@@ -4245,7 +4233,7 @@
         <v>7</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D220" s="1">
         <v>0.78539999999999999</v>
@@ -4262,7 +4250,7 @@
         <v>5</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D221" s="1">
         <v>0.90800000000000003</v>
@@ -4279,7 +4267,7 @@
         <v>5</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D222" s="1">
         <v>0.90869999999999995</v>
@@ -4296,7 +4284,7 @@
         <v>5</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D223" s="1">
         <v>0.21560000000000001</v>
@@ -4310,10 +4298,10 @@
         <v>0</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D224" s="1">
         <v>0.23139999999999999</v>
@@ -4327,10 +4315,10 @@
         <v>0</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D225" s="1">
         <v>0.56430000000000002</v>
@@ -4344,10 +4332,10 @@
         <v>0</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D226" s="1">
         <v>0.56430000000000002</v>
@@ -4361,10 +4349,10 @@
         <v>0</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D227" s="1">
         <v>0.4672</v>
@@ -4378,10 +4366,10 @@
         <v>0</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D228" s="1">
         <v>0.23139999999999999</v>
@@ -4395,10 +4383,10 @@
         <v>0</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D229" s="1">
         <v>0.35670000000000002</v>
@@ -4412,10 +4400,10 @@
         <v>0</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D230" s="1">
         <v>0.23139999999999999</v>
@@ -4432,7 +4420,7 @@
         <v>2</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D231" s="1">
         <v>0.78539999999999999</v>
@@ -4446,10 +4434,10 @@
         <v>0</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D232" s="1">
         <v>0.1356</v>
@@ -4463,10 +4451,10 @@
         <v>0</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D233" s="1">
         <v>0.52339999999999998</v>
@@ -4480,10 +4468,10 @@
         <v>0</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D234" s="1">
         <v>7.6799999999999993E-2</v>
@@ -4497,10 +4485,10 @@
         <v>0</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D235" s="1">
         <v>0.3453</v>
@@ -4514,10 +4502,10 @@
         <v>0</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D236" s="1">
         <v>0.3453</v>
@@ -4531,10 +4519,10 @@
         <v>0</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D237" s="1">
         <v>0.3453</v>
@@ -4548,10 +4536,10 @@
         <v>0</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D238" s="1">
         <v>0.3453</v>
@@ -4565,10 +4553,10 @@
         <v>0</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D239" s="1">
         <v>0.78539999999999999</v>
@@ -4585,7 +4573,7 @@
         <v>1</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D240" s="1">
         <v>0.1983</v>
@@ -4602,7 +4590,7 @@
         <v>2</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D241" s="1">
         <v>0.78539999999999999</v>
@@ -4619,7 +4607,7 @@
         <v>1</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D242" s="1">
         <v>0.1983</v>
@@ -4636,7 +4624,7 @@
         <v>3</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D243" s="1">
         <v>0.78539999999999999</v>
@@ -4653,7 +4641,7 @@
         <v>1</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D244" s="1">
         <v>0.78539999999999999</v>
@@ -4670,7 +4658,7 @@
         <v>1</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D245" s="1">
         <v>0.3453</v>
@@ -4687,7 +4675,7 @@
         <v>2</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D246" s="1">
         <v>0.78539999999999999</v>
@@ -4704,7 +4692,7 @@
         <v>5</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D247" s="1">
         <v>0.54369999999999996</v>
@@ -4721,7 +4709,7 @@
         <v>1</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D248" s="1">
         <v>0.98560000000000003</v>
@@ -4738,7 +4726,7 @@
         <v>1</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D249" s="1">
         <v>0.98560000000000003</v>
@@ -4755,7 +4743,7 @@
         <v>2</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D250" s="1">
         <v>0.78539999999999999</v>
@@ -4772,7 +4760,7 @@
         <v>6</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D251" s="1">
         <v>0.78539999999999999</v>
@@ -4789,7 +4777,7 @@
         <v>3</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D252" s="1">
         <v>0.78539999999999999</v>
@@ -4806,7 +4794,7 @@
         <v>2</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D253" s="1">
         <v>0.78539999999999999</v>
@@ -4823,7 +4811,7 @@
         <v>3</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D254" s="1">
         <v>0.78539999999999999</v>
@@ -4840,7 +4828,7 @@
         <v>6</v>
       </c>
       <c r="C255" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D255" s="1">
         <v>0.78539999999999999</v>
@@ -4857,7 +4845,7 @@
         <v>5</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D256" s="1">
         <v>0.98560000000000003</v>
@@ -4874,7 +4862,7 @@
         <v>1</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D257" s="1">
         <v>0.12559999999999999</v>
@@ -4891,7 +4879,7 @@
         <v>3</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D258" s="1">
         <v>0.78539999999999999</v>
@@ -4908,7 +4896,7 @@
         <v>5</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D259" s="1">
         <v>0.43759999999999999</v>
@@ -4925,7 +4913,7 @@
         <v>3</v>
       </c>
       <c r="C260" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D260" s="1">
         <v>0.78539999999999999</v>
@@ -4942,7 +4930,7 @@
         <v>2</v>
       </c>
       <c r="C261" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D261" s="1">
         <v>0.78539999999999999</v>
@@ -4959,7 +4947,7 @@
         <v>5</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D262" s="1">
         <v>0.76890000000000003</v>
@@ -4976,7 +4964,7 @@
         <v>7</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D263" s="1">
         <v>0.34560000000000002</v>
@@ -4993,7 +4981,7 @@
         <v>2</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D264" s="1">
         <v>0.24560000000000001</v>
@@ -5010,7 +4998,7 @@
         <v>3</v>
       </c>
       <c r="C265" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D265" s="1">
         <v>0.13239999999999999</v>
@@ -5027,7 +5015,7 @@
         <v>5</v>
       </c>
       <c r="C266" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D266" s="1">
         <v>0.23139999999999999</v>
@@ -5044,7 +5032,7 @@
         <v>5</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D267" s="1">
         <v>0.23139999999999999</v>
@@ -5061,7 +5049,7 @@
         <v>7</v>
       </c>
       <c r="C268" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D268" s="1">
         <v>0.23139999999999999</v>
@@ -5078,7 +5066,7 @@
         <v>3</v>
       </c>
       <c r="C269" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D269" s="1">
         <v>0.23139999999999999</v>
@@ -5095,7 +5083,7 @@
         <v>6</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D270" s="1">
         <v>0.35670000000000002</v>
@@ -5112,7 +5100,7 @@
         <v>6</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D271" s="1">
         <v>0.23139999999999999</v>
@@ -5129,7 +5117,7 @@
         <v>2</v>
       </c>
       <c r="C272" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D272" s="1">
         <v>0.1356</v>
@@ -5146,7 +5134,7 @@
         <v>6</v>
       </c>
       <c r="C273" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D273" s="1">
         <v>7.6799999999999993E-2</v>
@@ -5163,7 +5151,7 @@
         <v>2</v>
       </c>
       <c r="C274" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D274" s="1">
         <v>0.3453</v>
@@ -5180,7 +5168,7 @@
         <v>3</v>
       </c>
       <c r="C275" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D275" s="1">
         <v>0.3453</v>
@@ -5197,7 +5185,7 @@
         <v>6</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D276" s="1">
         <v>0.3453</v>
@@ -5214,7 +5202,7 @@
         <v>5</v>
       </c>
       <c r="C277" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D277" s="1">
         <v>0.3453</v>
@@ -5231,7 +5219,7 @@
         <v>3</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D278" s="1">
         <v>0.3453</v>
@@ -5248,7 +5236,7 @@
         <v>1</v>
       </c>
       <c r="C279" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D279" s="1">
         <v>0.54369999999999996</v>
@@ -5265,7 +5253,7 @@
         <v>1</v>
       </c>
       <c r="C280" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D280" s="1">
         <v>0.98560000000000003</v>
@@ -5282,7 +5270,7 @@
         <v>5</v>
       </c>
       <c r="C281" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D281" s="1">
         <v>0.98560000000000003</v>
@@ -5299,7 +5287,7 @@
         <v>5</v>
       </c>
       <c r="C282" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D282" s="1">
         <v>0.98560000000000003</v>
@@ -5316,7 +5304,7 @@
         <v>2</v>
       </c>
       <c r="C283" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D283" s="1">
         <v>0.12559999999999999</v>
@@ -5333,7 +5321,7 @@
         <v>2</v>
       </c>
       <c r="C284" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D284" s="1">
         <v>0.43759999999999999</v>
@@ -5350,7 +5338,7 @@
         <v>2</v>
       </c>
       <c r="C285" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D285" s="1">
         <v>0.3256</v>
@@ -5367,7 +5355,7 @@
         <v>2</v>
       </c>
       <c r="C286" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D286" s="1">
         <v>0.14560000000000001</v>
@@ -5384,7 +5372,7 @@
         <v>7</v>
       </c>
       <c r="C287" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D287" s="1">
         <v>0.78539999999999999</v>
@@ -5401,7 +5389,7 @@
         <v>1</v>
       </c>
       <c r="C288" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D288" s="1">
         <v>0.23949999999999999</v>
@@ -5418,7 +5406,7 @@
         <v>5</v>
       </c>
       <c r="C289" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D289" s="1">
         <v>0.78539999999999999</v>
@@ -5435,7 +5423,7 @@
         <v>2</v>
       </c>
       <c r="C290" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D290" s="1">
         <v>1.0057</v>
@@ -5452,7 +5440,7 @@
         <v>2</v>
       </c>
       <c r="C291" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D291" s="1">
         <v>1.0057</v>
@@ -5469,7 +5457,7 @@
         <v>2</v>
       </c>
       <c r="C292" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D292" s="1">
         <v>1.0057</v>
@@ -5486,7 +5474,7 @@
         <v>1</v>
       </c>
       <c r="C293" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D293" s="1">
         <v>0.23949999999999999</v>
@@ -5503,7 +5491,7 @@
         <v>5</v>
       </c>
       <c r="C294" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D294" s="1">
         <v>1.0057</v>
@@ -5520,7 +5508,7 @@
         <v>5</v>
       </c>
       <c r="C295" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D295" s="1">
         <v>1.0057</v>
@@ -5537,7 +5525,7 @@
         <v>7</v>
       </c>
       <c r="C296" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D296" s="1">
         <v>1.0057</v>
@@ -5554,7 +5542,7 @@
         <v>2</v>
       </c>
       <c r="C297" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D297" s="1">
         <v>1.0057</v>
@@ -5571,7 +5559,7 @@
         <v>3</v>
       </c>
       <c r="C298" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D298" s="1">
         <v>0.23449999999999999</v>
@@ -5588,7 +5576,7 @@
         <v>5</v>
       </c>
       <c r="C299" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D299" s="1">
         <v>1.0057</v>
@@ -5605,7 +5593,7 @@
         <v>2</v>
       </c>
       <c r="C300" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D300" s="1">
         <v>1.0057</v>
@@ -5622,7 +5610,7 @@
         <v>2</v>
       </c>
       <c r="C301" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D301" s="1">
         <v>1.0057</v>
@@ -5639,7 +5627,7 @@
         <v>2</v>
       </c>
       <c r="C302" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D302" s="1">
         <v>1.0057</v>
@@ -5656,7 +5644,7 @@
         <v>2</v>
       </c>
       <c r="C303" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D303" s="1">
         <v>1.0057</v>
@@ -5673,7 +5661,7 @@
         <v>3</v>
       </c>
       <c r="C304" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D304" s="1">
         <v>0.23449999999999999</v>
@@ -5690,7 +5678,7 @@
         <v>2</v>
       </c>
       <c r="C305" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D305" s="1">
         <v>1.0057</v>
@@ -5707,7 +5695,7 @@
         <v>2</v>
       </c>
       <c r="C306" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D306" s="1">
         <v>1.0057</v>
@@ -5724,7 +5712,7 @@
         <v>2</v>
       </c>
       <c r="C307" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D307" s="1">
         <v>1.0057</v>
@@ -5741,7 +5729,7 @@
         <v>2</v>
       </c>
       <c r="C308" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D308" s="1">
         <v>1.0057</v>
@@ -5758,7 +5746,7 @@
         <v>3</v>
       </c>
       <c r="C309" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D309" s="1">
         <v>0.23449999999999999</v>
@@ -5775,7 +5763,7 @@
         <v>2</v>
       </c>
       <c r="C310" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D310" s="1">
         <v>1.0057</v>
@@ -5792,7 +5780,7 @@
         <v>2</v>
       </c>
       <c r="C311" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D311" s="1">
         <v>0.75319999999999998</v>
@@ -5809,7 +5797,7 @@
         <v>3</v>
       </c>
       <c r="C312" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D312" s="1">
         <v>0.75319999999999998</v>
@@ -5826,7 +5814,7 @@
         <v>3</v>
       </c>
       <c r="C313" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D313" s="1">
         <v>0.75319999999999998</v>
@@ -5843,7 +5831,7 @@
         <v>3</v>
       </c>
       <c r="C314" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D314" s="1">
         <v>0.75319999999999998</v>
@@ -5860,7 +5848,7 @@
         <v>3</v>
       </c>
       <c r="C315" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D315" s="1">
         <v>0.75319999999999998</v>
@@ -5877,7 +5865,7 @@
         <v>3</v>
       </c>
       <c r="C316" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D316" s="1">
         <v>0.75319999999999998</v>
@@ -5894,7 +5882,7 @@
         <v>3</v>
       </c>
       <c r="C317" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D317" s="1">
         <v>0.86539999999999995</v>
@@ -5911,7 +5899,7 @@
         <v>3</v>
       </c>
       <c r="C318" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D318" s="1">
         <v>0.86539999999999995</v>
@@ -5928,7 +5916,7 @@
         <v>3</v>
       </c>
       <c r="C319" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D319" s="1">
         <v>0.86539999999999995</v>
@@ -5945,7 +5933,7 @@
         <v>2</v>
       </c>
       <c r="C320" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D320" s="1">
         <v>0.86539999999999995</v>
@@ -5962,7 +5950,7 @@
         <v>2</v>
       </c>
       <c r="C321" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D321" s="1">
         <v>0.86539999999999995</v>
@@ -5979,7 +5967,7 @@
         <v>2</v>
       </c>
       <c r="C322" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D322" s="1">
         <v>0.86539999999999995</v>
@@ -5996,7 +5984,7 @@
         <v>2</v>
       </c>
       <c r="C323" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D323" s="1">
         <v>0.86539999999999995</v>
@@ -6013,7 +6001,7 @@
         <v>3</v>
       </c>
       <c r="C324" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D324" s="1">
         <v>0.86539999999999995</v>
@@ -6030,7 +6018,7 @@
         <v>7</v>
       </c>
       <c r="C325" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D325" s="1">
         <v>0.86539999999999995</v>
@@ -6047,7 +6035,7 @@
         <v>7</v>
       </c>
       <c r="C326" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D326" s="1">
         <v>0.97560000000000002</v>
@@ -6064,7 +6052,7 @@
         <v>7</v>
       </c>
       <c r="C327" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D327" s="1">
         <v>0.97560000000000002</v>
@@ -6081,7 +6069,7 @@
         <v>7</v>
       </c>
       <c r="C328" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D328" s="1">
         <v>0.97560000000000002</v>
@@ -6098,7 +6086,7 @@
         <v>7</v>
       </c>
       <c r="C329" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D329" s="1">
         <v>0.97560000000000002</v>
@@ -6115,7 +6103,7 @@
         <v>7</v>
       </c>
       <c r="C330" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D330" s="1">
         <v>0.97560000000000002</v>
@@ -6132,7 +6120,7 @@
         <v>7</v>
       </c>
       <c r="C331" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D331" s="1">
         <v>0.97560000000000002</v>
@@ -6149,7 +6137,7 @@
         <v>7</v>
       </c>
       <c r="C332" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D332" s="1">
         <v>0.97560000000000002</v>
@@ -6166,7 +6154,7 @@
         <v>7</v>
       </c>
       <c r="C333" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D333" s="1">
         <v>0.76029999999999998</v>
@@ -6183,7 +6171,7 @@
         <v>7</v>
       </c>
       <c r="C334" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D334" s="1">
         <v>0.76029999999999998</v>
@@ -6200,7 +6188,7 @@
         <v>3</v>
       </c>
       <c r="C335" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D335" s="1">
         <v>0.76029999999999998</v>
@@ -6217,7 +6205,7 @@
         <v>7</v>
       </c>
       <c r="C336" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D336" s="1">
         <v>0.76029999999999998</v>
@@ -6234,7 +6222,7 @@
         <v>7</v>
       </c>
       <c r="C337" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D337" s="1">
         <v>0.76029999999999998</v>
@@ -6251,7 +6239,7 @@
         <v>7</v>
       </c>
       <c r="C338" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D338" s="1">
         <v>0.76029999999999998</v>
@@ -6268,7 +6256,7 @@
         <v>7</v>
       </c>
       <c r="C339" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D339" s="1">
         <v>0.76029999999999998</v>
@@ -6285,7 +6273,7 @@
         <v>7</v>
       </c>
       <c r="C340" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D340" s="1">
         <v>0.85780000000000001</v>
@@ -6302,7 +6290,7 @@
         <v>6</v>
       </c>
       <c r="C341" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D341" s="1">
         <v>0.85780000000000001</v>
@@ -6319,7 +6307,7 @@
         <v>7</v>
       </c>
       <c r="C342" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D342" s="1">
         <v>0.85780000000000001</v>
@@ -6336,7 +6324,7 @@
         <v>5</v>
       </c>
       <c r="C343" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D343" s="1">
         <v>0.85780000000000001</v>
@@ -6353,7 +6341,7 @@
         <v>7</v>
       </c>
       <c r="C344" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D344" s="1">
         <v>0.85780000000000001</v>
@@ -6370,7 +6358,7 @@
         <v>3</v>
       </c>
       <c r="C345" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D345" s="1">
         <v>0.85780000000000001</v>
@@ -6387,7 +6375,7 @@
         <v>7</v>
       </c>
       <c r="C346" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D346" s="1">
         <v>0.91449999999999998</v>
@@ -6404,7 +6392,7 @@
         <v>7</v>
       </c>
       <c r="C347" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D347" s="1">
         <v>0.91449999999999998</v>
@@ -6421,7 +6409,7 @@
         <v>7</v>
       </c>
       <c r="C348" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D348" s="1">
         <v>0.91449999999999998</v>
@@ -6438,7 +6426,7 @@
         <v>7</v>
       </c>
       <c r="C349" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D349" s="1">
         <v>0.91449999999999998</v>
@@ -6455,7 +6443,7 @@
         <v>5</v>
       </c>
       <c r="C350" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D350" s="1">
         <v>0.91449999999999998</v>
@@ -6472,7 +6460,7 @@
         <v>7</v>
       </c>
       <c r="C351" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D351" s="1">
         <v>0.91449999999999998</v>
@@ -6489,7 +6477,7 @@
         <v>7</v>
       </c>
       <c r="C352" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D352" s="1">
         <v>0.91449999999999998</v>
@@ -6506,7 +6494,7 @@
         <v>7</v>
       </c>
       <c r="C353" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D353" s="1">
         <v>0.91449999999999998</v>
@@ -6523,7 +6511,7 @@
         <v>7</v>
       </c>
       <c r="C354" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D354" s="1">
         <v>0.91449999999999998</v>
@@ -6540,7 +6528,7 @@
         <v>7</v>
       </c>
       <c r="C355" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D355" s="1">
         <v>0.91449999999999998</v>
@@ -6557,7 +6545,7 @@
         <v>7</v>
       </c>
       <c r="C356" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D356" s="1">
         <v>0.91449999999999998</v>
@@ -6574,7 +6562,7 @@
         <v>7</v>
       </c>
       <c r="C357" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D357" s="1">
         <v>0.91449999999999998</v>
@@ -6591,7 +6579,7 @@
         <v>7</v>
       </c>
       <c r="C358" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D358" s="1">
         <v>0.91449999999999998</v>
@@ -6608,7 +6596,7 @@
         <v>2</v>
       </c>
       <c r="C359" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D359" s="1">
         <v>0.91449999999999998</v>
@@ -6625,7 +6613,7 @@
         <v>6</v>
       </c>
       <c r="C360" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D360" s="1">
         <v>0.91449999999999998</v>
@@ -6642,7 +6630,7 @@
         <v>3</v>
       </c>
       <c r="C361" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D361" s="1">
         <v>0.78900000000000003</v>
@@ -6659,7 +6647,7 @@
         <v>5</v>
       </c>
       <c r="C362" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D362" s="1">
         <v>0.78900000000000003</v>
@@ -6676,7 +6664,7 @@
         <v>5</v>
       </c>
       <c r="C363" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D363" s="1">
         <v>0.78900000000000003</v>
@@ -6693,7 +6681,7 @@
         <v>5</v>
       </c>
       <c r="C364" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D364" s="1">
         <v>0.78900000000000003</v>
@@ -6710,7 +6698,7 @@
         <v>3</v>
       </c>
       <c r="C365" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D365" s="1">
         <v>0.78900000000000003</v>
@@ -6727,7 +6715,7 @@
         <v>3</v>
       </c>
       <c r="C366" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D366" s="1">
         <v>0.78900000000000003</v>
@@ -6744,7 +6732,7 @@
         <v>7</v>
       </c>
       <c r="C367" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D367" s="1">
         <v>0.78900000000000003</v>
@@ -6761,7 +6749,7 @@
         <v>7</v>
       </c>
       <c r="C368" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D368" s="1">
         <v>0.65429999999999999</v>
@@ -6778,7 +6766,7 @@
         <v>7</v>
       </c>
       <c r="C369" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D369" s="1">
         <v>0.65429999999999999</v>
@@ -6795,7 +6783,7 @@
         <v>7</v>
       </c>
       <c r="C370" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D370" s="1">
         <v>0.65429999999999999</v>
@@ -6812,7 +6800,7 @@
         <v>7</v>
       </c>
       <c r="C371" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D371" s="1">
         <v>0.65429999999999999</v>
@@ -6829,7 +6817,7 @@
         <v>7</v>
       </c>
       <c r="C372" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D372" s="1">
         <v>0.65429999999999999</v>
@@ -6846,7 +6834,7 @@
         <v>7</v>
       </c>
       <c r="C373" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D373" s="1">
         <v>0.65429999999999999</v>
@@ -6863,7 +6851,7 @@
         <v>7</v>
       </c>
       <c r="C374" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D374" s="1">
         <v>0.65429999999999999</v>
@@ -6880,7 +6868,7 @@
         <v>7</v>
       </c>
       <c r="C375" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D375" s="1">
         <v>0.53459999999999996</v>
@@ -6897,7 +6885,7 @@
         <v>7</v>
       </c>
       <c r="C376" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D376" s="1">
         <v>0.53459999999999996</v>
@@ -6914,7 +6902,7 @@
         <v>7</v>
       </c>
       <c r="C377" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D377" s="1">
         <v>0.53459999999999996</v>
@@ -6931,7 +6919,7 @@
         <v>7</v>
       </c>
       <c r="C378" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D378" s="1">
         <v>0.53459999999999996</v>
@@ -6948,7 +6936,7 @@
         <v>7</v>
       </c>
       <c r="C379" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D379" s="1">
         <v>0.53459999999999996</v>
@@ -6965,7 +6953,7 @@
         <v>3</v>
       </c>
       <c r="C380" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D380" s="1">
         <v>0.23449999999999999</v>
@@ -6982,7 +6970,7 @@
         <v>3</v>
       </c>
       <c r="C381" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D381" s="1">
         <v>0.23449999999999999</v>
@@ -6999,7 +6987,7 @@
         <v>2</v>
       </c>
       <c r="C382" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D382" s="1">
         <v>0.53459999999999996</v>
@@ -7016,7 +7004,7 @@
         <v>2</v>
       </c>
       <c r="C383" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D383" s="1">
         <v>0.53459999999999996</v>
@@ -7033,7 +7021,7 @@
         <v>3</v>
       </c>
       <c r="C384" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D384" s="1">
         <v>0.23449999999999999</v>
@@ -7050,7 +7038,7 @@
         <v>3</v>
       </c>
       <c r="C385" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D385" s="1">
         <v>0.23449999999999999</v>
@@ -7067,7 +7055,7 @@
         <v>7</v>
       </c>
       <c r="C386" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D386" s="1">
         <v>0.78649999999999998</v>
@@ -7084,7 +7072,7 @@
         <v>3</v>
       </c>
       <c r="C387" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D387" s="1">
         <v>0.23449999999999999</v>
@@ -7101,7 +7089,7 @@
         <v>7</v>
       </c>
       <c r="C388" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D388" s="1">
         <v>0.78649999999999998</v>
@@ -7118,7 +7106,7 @@
         <v>7</v>
       </c>
       <c r="C389" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D389" s="1">
         <v>0.78649999999999998</v>
@@ -7135,7 +7123,7 @@
         <v>3</v>
       </c>
       <c r="C390" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D390" s="1">
         <v>0.54359999999999997</v>
@@ -7152,7 +7140,7 @@
         <v>7</v>
       </c>
       <c r="C391" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D391" s="1">
         <v>0.54359999999999997</v>
@@ -7169,7 +7157,7 @@
         <v>7</v>
       </c>
       <c r="C392" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D392" s="1">
         <v>0.54359999999999997</v>
@@ -7186,7 +7174,7 @@
         <v>7</v>
       </c>
       <c r="C393" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D393" s="1">
         <v>0.54359999999999997</v>
@@ -7203,7 +7191,7 @@
         <v>7</v>
       </c>
       <c r="C394" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D394" s="1">
         <v>0.54359999999999997</v>
@@ -7220,7 +7208,7 @@
         <v>7</v>
       </c>
       <c r="C395" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D395" s="1">
         <v>0.54359999999999997</v>
@@ -7237,7 +7225,7 @@
         <v>7</v>
       </c>
       <c r="C396" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D396" s="1">
         <v>0.67889999999999995</v>
@@ -7254,7 +7242,7 @@
         <v>7</v>
       </c>
       <c r="C397" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D397" s="1">
         <v>0.75670000000000004</v>
@@ -7271,7 +7259,7 @@
         <v>7</v>
       </c>
       <c r="C398" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D398" s="1">
         <v>0.75670000000000004</v>
@@ -7288,7 +7276,7 @@
         <v>2</v>
       </c>
       <c r="C399" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D399" s="1">
         <v>0.23449999999999999</v>
@@ -7305,7 +7293,7 @@
         <v>6</v>
       </c>
       <c r="C400" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D400" s="1">
         <v>0.75670000000000004</v>
@@ -7322,7 +7310,7 @@
         <v>3</v>
       </c>
       <c r="C401" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D401" s="1">
         <v>0.75670000000000004</v>
@@ -7339,7 +7327,7 @@
         <v>5</v>
       </c>
       <c r="C402" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D402" s="1">
         <v>0.65459999999999996</v>
@@ -7356,7 +7344,7 @@
         <v>5</v>
       </c>
       <c r="C403" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D403" s="1">
         <v>0.65459999999999996</v>
@@ -7373,7 +7361,7 @@
         <v>5</v>
       </c>
       <c r="C404" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D404" s="1">
         <v>0.65459999999999996</v>
@@ -7390,7 +7378,7 @@
         <v>3</v>
       </c>
       <c r="C405" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D405" s="1">
         <v>0.25669999999999998</v>
@@ -7407,7 +7395,7 @@
         <v>3</v>
       </c>
       <c r="C406" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D406" s="1">
         <v>0.23449999999999999</v>
@@ -7424,7 +7412,7 @@
         <v>7</v>
       </c>
       <c r="C407" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D407" s="1">
         <v>0.65459999999999996</v>
@@ -7441,7 +7429,7 @@
         <v>7</v>
       </c>
       <c r="C408" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D408" s="1">
         <v>0.65459999999999996</v>
@@ -7458,7 +7446,7 @@
         <v>7</v>
       </c>
       <c r="C409" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D409" s="1">
         <v>0.6754</v>
@@ -7475,7 +7463,7 @@
         <v>7</v>
       </c>
       <c r="C410" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D410" s="1">
         <v>0.65459999999999996</v>
@@ -7492,7 +7480,7 @@
         <v>3</v>
       </c>
       <c r="C411" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D411" s="1">
         <v>0.23449999999999999</v>
@@ -7509,7 +7497,7 @@
         <v>7</v>
       </c>
       <c r="C412" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D412" s="1">
         <v>0.65459999999999996</v>
@@ -7526,7 +7514,7 @@
         <v>7</v>
       </c>
       <c r="C413" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D413" s="1">
         <v>0.65459999999999996</v>
@@ -7543,7 +7531,7 @@
         <v>7</v>
       </c>
       <c r="C414" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D414" s="1">
         <v>0.78559999999999997</v>
@@ -7560,7 +7548,7 @@
         <v>3</v>
       </c>
       <c r="C415" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D415" s="1">
         <v>0.23449999999999999</v>
@@ -7577,7 +7565,7 @@
         <v>7</v>
       </c>
       <c r="C416" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D416" s="1">
         <v>0.65459999999999996</v>
@@ -7594,7 +7582,7 @@
         <v>7</v>
       </c>
       <c r="C417" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D417" s="1">
         <v>0.75670000000000004</v>
@@ -7611,7 +7599,7 @@
         <v>7</v>
       </c>
       <c r="C418" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D418" s="1">
         <v>0.75670000000000004</v>
@@ -7628,7 +7616,7 @@
         <v>7</v>
       </c>
       <c r="C419" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D419" s="1">
         <v>0.75670000000000004</v>
@@ -7645,7 +7633,7 @@
         <v>2</v>
       </c>
       <c r="C420" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D420" s="1">
         <v>0.28449999999999998</v>
@@ -7662,7 +7650,7 @@
         <v>1</v>
       </c>
       <c r="C421" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D421" s="1">
         <v>0.23949999999999999</v>
@@ -7679,7 +7667,7 @@
         <v>2</v>
       </c>
       <c r="C422" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D422" s="1">
         <v>0.23449999999999999</v>
@@ -7696,7 +7684,7 @@
         <v>2</v>
       </c>
       <c r="C423" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D423" s="1">
         <v>0.23449999999999999</v>
@@ -7713,7 +7701,7 @@
         <v>6</v>
       </c>
       <c r="C424" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D424" s="1">
         <v>0.75670000000000004</v>
@@ -7730,7 +7718,7 @@
         <v>3</v>
       </c>
       <c r="C425" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D425" s="1">
         <v>0.23449999999999999</v>
@@ -7747,7 +7735,7 @@
         <v>2</v>
       </c>
       <c r="C426" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D426" s="1">
         <v>0.23449999999999999</v>
@@ -7764,7 +7752,7 @@
         <v>2</v>
       </c>
       <c r="C427" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D427" s="1">
         <v>0.23449999999999999</v>
@@ -7781,7 +7769,7 @@
         <v>2</v>
       </c>
       <c r="C428" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D428" s="1">
         <v>0.23449999999999999</v>
@@ -7798,7 +7786,7 @@
         <v>7</v>
       </c>
       <c r="C429" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D429" s="1">
         <v>0.75670000000000004</v>
@@ -7815,7 +7803,7 @@
         <v>1</v>
       </c>
       <c r="C430" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D430" s="1">
         <v>0.23150000000000001</v>
@@ -7832,7 +7820,7 @@
         <v>2</v>
       </c>
       <c r="C431" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D431" s="1">
         <v>0.23449999999999999</v>
@@ -7849,7 +7837,7 @@
         <v>1</v>
       </c>
       <c r="C432" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D432" s="1">
         <v>0.23949999999999999</v>
@@ -7866,7 +7854,7 @@
         <v>3</v>
       </c>
       <c r="C433" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D433" s="1">
         <v>0.23449999999999999</v>
@@ -7883,7 +7871,7 @@
         <v>1</v>
       </c>
       <c r="C434" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D434" s="1">
         <v>0.23050000000000001</v>
@@ -7900,7 +7888,7 @@
         <v>1</v>
       </c>
       <c r="C435" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D435" s="1">
         <v>0.23949999999999999</v>
@@ -7917,7 +7905,7 @@
         <v>2</v>
       </c>
       <c r="C436" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D436" s="1">
         <v>0.23449999999999999</v>
@@ -7934,7 +7922,7 @@
         <v>5</v>
       </c>
       <c r="C437" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D437" s="1">
         <v>0.75670000000000004</v>
@@ -7951,7 +7939,7 @@
         <v>1</v>
       </c>
       <c r="C438" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D438" s="1">
         <v>0.22950000000000001</v>
@@ -7968,7 +7956,7 @@
         <v>1</v>
       </c>
       <c r="C439" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D439" s="1">
         <v>0.23949999999999999</v>
@@ -7985,7 +7973,7 @@
         <v>2</v>
       </c>
       <c r="C440" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D440" s="1">
         <v>0.23449999999999999</v>
@@ -8002,7 +7990,7 @@
         <v>6</v>
       </c>
       <c r="C441" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D441" s="1">
         <v>0.5645</v>
@@ -8019,7 +8007,7 @@
         <v>5</v>
       </c>
       <c r="C442" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D442" s="1">
         <v>0.5645</v>
@@ -8036,7 +8024,7 @@
         <v>2</v>
       </c>
       <c r="C443" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D443" s="1">
         <v>0.23449999999999999</v>
@@ -8053,7 +8041,7 @@
         <v>3</v>
       </c>
       <c r="C444" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D444" s="1">
         <v>0.23449999999999999</v>
@@ -8070,7 +8058,7 @@
         <v>6</v>
       </c>
       <c r="C445" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D445" s="1">
         <v>0.5645</v>
@@ -8087,7 +8075,7 @@
         <v>5</v>
       </c>
       <c r="C446" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D446" s="1">
         <v>0.5645</v>
@@ -8104,7 +8092,7 @@
         <v>1</v>
       </c>
       <c r="C447" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D447" s="1">
         <v>1.2344999999999999</v>
@@ -8121,7 +8109,7 @@
         <v>3</v>
       </c>
       <c r="C448" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D448" s="1">
         <v>0.23449999999999999</v>
@@ -8138,7 +8126,7 @@
         <v>5</v>
       </c>
       <c r="C449" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D449" s="1">
         <v>0.23449999999999999</v>
@@ -8155,7 +8143,7 @@
         <v>5</v>
       </c>
       <c r="C450" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D450" s="1">
         <v>0.23449999999999999</v>
@@ -8172,7 +8160,7 @@
         <v>2</v>
       </c>
       <c r="C451" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D451" s="1">
         <v>0.23449999999999999</v>
@@ -8189,7 +8177,7 @@
         <v>5</v>
       </c>
       <c r="C452" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D452" s="1">
         <v>0.23449999999999999</v>
@@ -8206,7 +8194,7 @@
         <v>7</v>
       </c>
       <c r="C453" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D453" s="1">
         <v>0.5645</v>
@@ -8223,7 +8211,7 @@
         <v>2</v>
       </c>
       <c r="C454" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D454" s="1">
         <v>0.5645</v>
@@ -8240,7 +8228,7 @@
         <v>5</v>
       </c>
       <c r="C455" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D455" s="1">
         <v>0.5645</v>
@@ -8257,7 +8245,7 @@
         <v>5</v>
       </c>
       <c r="C456" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D456" s="1">
         <v>0.78539999999999999</v>
@@ -8274,7 +8262,7 @@
         <v>5</v>
       </c>
       <c r="C457" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D457" s="1">
         <v>0.15429999999999999</v>
@@ -8291,7 +8279,7 @@
         <v>7</v>
       </c>
       <c r="C458" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D458" s="1">
         <v>0.3256</v>
@@ -8308,7 +8296,7 @@
         <v>5</v>
       </c>
       <c r="C459" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D459" s="1">
         <v>0.23449999999999999</v>
@@ -8325,7 +8313,7 @@
         <v>5</v>
       </c>
       <c r="C460" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D460" s="1">
         <v>0.23449999999999999</v>
@@ -8342,7 +8330,7 @@
         <v>5</v>
       </c>
       <c r="C461" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D461" s="1">
         <v>0.23449999999999999</v>
@@ -8356,10 +8344,10 @@
         <v>8</v>
       </c>
       <c r="B462" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C462" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D462" s="1">
         <v>0.23449999999999999</v>
@@ -8373,10 +8361,10 @@
         <v>8</v>
       </c>
       <c r="B463" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C463" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D463" s="1">
         <v>0.79890000000000005</v>
@@ -8390,10 +8378,10 @@
         <v>8</v>
       </c>
       <c r="B464" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C464" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D464" s="1">
         <v>0.2356</v>
@@ -8407,10 +8395,10 @@
         <v>8</v>
       </c>
       <c r="B465" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C465" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D465" s="1">
         <v>0.75490000000000002</v>
@@ -8424,10 +8412,10 @@
         <v>4</v>
       </c>
       <c r="B466" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C466" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D466" s="1">
         <v>0.58989999999999998</v>
@@ -8441,10 +8429,10 @@
         <v>4</v>
       </c>
       <c r="B467" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C467" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D467" s="1">
         <v>0.26889999999999997</v>
@@ -8458,10 +8446,10 @@
         <v>8</v>
       </c>
       <c r="B468" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C468" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D468" s="1">
         <v>0.5645</v>
@@ -8478,7 +8466,7 @@
         <v>2</v>
       </c>
       <c r="C469" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D469" s="1">
         <v>0.83450000000000002</v>
@@ -8495,7 +8483,7 @@
         <v>2</v>
       </c>
       <c r="C470" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D470" s="1">
         <v>0.83450000000000002</v>
@@ -8512,7 +8500,7 @@
         <v>6</v>
       </c>
       <c r="C471" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D471" s="1">
         <v>0.83450000000000002</v>
@@ -8529,7 +8517,7 @@
         <v>3</v>
       </c>
       <c r="C472" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D472" s="1">
         <v>0.83450000000000002</v>
@@ -8546,7 +8534,7 @@
         <v>2</v>
       </c>
       <c r="C473" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D473" s="1">
         <v>1.1055999999999999</v>
@@ -8563,7 +8551,7 @@
         <v>2</v>
       </c>
       <c r="C474" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D474" s="1">
         <v>1.1055999999999999</v>
@@ -8580,7 +8568,7 @@
         <v>2</v>
       </c>
       <c r="C475" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D475" s="1">
         <v>1.1055999999999999</v>
@@ -8597,7 +8585,7 @@
         <v>7</v>
       </c>
       <c r="C476" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D476" s="1">
         <v>1.1055999999999999</v>
@@ -8614,7 +8602,7 @@
         <v>1</v>
       </c>
       <c r="C477" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D477" s="1">
         <v>0.23949999999999999</v>
@@ -8631,7 +8619,7 @@
         <v>2</v>
       </c>
       <c r="C478" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D478" s="1">
         <v>0.56340000000000001</v>
@@ -8648,7 +8636,7 @@
         <v>1</v>
       </c>
       <c r="C479" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D479" s="1">
         <v>0.23949999999999999</v>
@@ -8665,7 +8653,7 @@
         <v>3</v>
       </c>
       <c r="C480" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D480" s="1">
         <v>0.56340000000000001</v>
@@ -8682,7 +8670,7 @@
         <v>1</v>
       </c>
       <c r="C481" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D481" s="1">
         <v>0.27750000000000002</v>
@@ -8699,7 +8687,7 @@
         <v>1</v>
       </c>
       <c r="C482" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D482" s="1">
         <v>1.2395</v>
@@ -8716,7 +8704,7 @@
         <v>2</v>
       </c>
       <c r="C483" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D483" s="1">
         <v>0.56340000000000001</v>
@@ -8733,7 +8721,7 @@
         <v>5</v>
       </c>
       <c r="C484" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D484" s="1">
         <v>0.23449999999999999</v>
@@ -8750,7 +8738,7 @@
         <v>1</v>
       </c>
       <c r="C485" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D485" s="1">
         <v>0.23949999999999999</v>
@@ -8767,7 +8755,7 @@
         <v>1</v>
       </c>
       <c r="C486" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D486" s="1">
         <v>0.23949999999999999</v>
@@ -8784,7 +8772,7 @@
         <v>2</v>
       </c>
       <c r="C487" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D487" s="1">
         <v>0.23449999999999999</v>
@@ -8801,7 +8789,7 @@
         <v>6</v>
       </c>
       <c r="C488" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D488" s="1">
         <v>0.56340000000000001</v>
@@ -8818,7 +8806,7 @@
         <v>5</v>
       </c>
       <c r="C489" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D489" s="1">
         <v>0.56340000000000001</v>
@@ -8835,7 +8823,7 @@
         <v>2</v>
       </c>
       <c r="C490" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D490" s="1">
         <v>0.56340000000000001</v>
@@ -8852,7 +8840,7 @@
         <v>3</v>
       </c>
       <c r="C491" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D491" s="1">
         <v>0.76449999999999996</v>
@@ -8869,7 +8857,7 @@
         <v>6</v>
       </c>
       <c r="C492" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D492" s="1">
         <v>0.45669999999999999</v>
@@ -8886,7 +8874,7 @@
         <v>5</v>
       </c>
       <c r="C493" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D493" s="1">
         <v>0.1234</v>
@@ -8903,7 +8891,7 @@
         <v>1</v>
       </c>
       <c r="C494" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D494" s="1">
         <v>0.23949999999999999</v>
@@ -8920,7 +8908,7 @@
         <v>3</v>
       </c>
       <c r="C495" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D495" s="1">
         <v>0.23449999999999999</v>
@@ -8937,7 +8925,7 @@
         <v>5</v>
       </c>
       <c r="C496" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D496" s="1">
         <v>0.23449999999999999</v>
@@ -8954,7 +8942,7 @@
         <v>5</v>
       </c>
       <c r="C497" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D497" s="1">
         <v>0.23449999999999999</v>
@@ -8971,7 +8959,7 @@
         <v>2</v>
       </c>
       <c r="C498" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D498" s="1">
         <v>0.25779999999999997</v>
@@ -8988,7 +8976,7 @@
         <v>5</v>
       </c>
       <c r="C499" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D499" s="1">
         <v>0.54210000000000003</v>
@@ -9005,7 +8993,7 @@
         <v>7</v>
       </c>
       <c r="C500" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D500" s="1">
         <v>0.25390000000000001</v>
@@ -9022,7 +9010,7 @@
         <v>2</v>
       </c>
       <c r="C501" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D501" s="1">
         <v>0.25990000000000002</v>
@@ -9039,7 +9027,7 @@
         <v>5</v>
       </c>
       <c r="C502" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D502" s="1">
         <v>0.2959</v>
@@ -9056,7 +9044,7 @@
         <v>5</v>
       </c>
       <c r="C503" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D503" s="1">
         <v>0.75019999999999998</v>
@@ -9073,7 +9061,7 @@
         <v>5</v>
       </c>
       <c r="C504" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D504" s="1">
         <v>0.75019999999999998</v>
@@ -9090,7 +9078,7 @@
         <v>5</v>
       </c>
       <c r="C505" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D505" s="1">
         <v>0.75019999999999998</v>

</xml_diff>